<commit_message>
Refactor ExcelSheetReader to have its own builder + refactoring testcases.
</commit_message>
<xml_diff>
--- a/src/test/resources/skipHiddenTestData.xlsx
+++ b/src/test/resources/skipHiddenTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E773D2C2-40CB-3447-A861-D7330AE42E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD76BCC7-4FFE-0A4A-B77C-82AC6C8AC8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="3520" windowWidth="25640" windowHeight="13480" firstSheet="5" activeTab="11" xr2:uid="{F0E37EA6-B81C-114C-AD9D-8AE6FA3EF7BF}"/>
+    <workbookView xWindow="2780" yWindow="3440" windowWidth="25640" windowHeight="13480" firstSheet="1" activeTab="7" xr2:uid="{F0E37EA6-B81C-114C-AD9D-8AE6FA3EF7BF}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseCase_Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Multi_Data" sheetId="11" r:id="rId11"/>
     <sheet name="Multi_Expected" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -764,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42594AB4-EFE5-204B-81AD-38E0779347C9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -837,8 +837,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7571C826-D0E5-C441-A8DD-7EE05C8C6CE6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more refactoring prep for upcoming optimization impl + hidden cell logic bug fix
</commit_message>
<xml_diff>
--- a/src/test/resources/skipHiddenTestData.xlsx
+++ b/src/test/resources/skipHiddenTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD76BCC7-4FFE-0A4A-B77C-82AC6C8AC8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF4CEF-012A-6D4E-9123-F4CC71630269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="3440" windowWidth="25640" windowHeight="13480" firstSheet="1" activeTab="7" xr2:uid="{F0E37EA6-B81C-114C-AD9D-8AE6FA3EF7BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" firstSheet="9" activeTab="12" xr2:uid="{F0E37EA6-B81C-114C-AD9D-8AE6FA3EF7BF}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseCase_Data" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     <sheet name="FirstLastColumn_Expected" sheetId="10" r:id="rId10"/>
     <sheet name="Multi_Data" sheetId="11" r:id="rId11"/>
     <sheet name="Multi_Expected" sheetId="12" r:id="rId12"/>
+    <sheet name="LastValueInvisible_Data" sheetId="13" r:id="rId13"/>
+    <sheet name="LastValueInvisible_Expected" sheetId="14" r:id="rId14"/>
+    <sheet name="LongestRowInvisible_Data" sheetId="15" r:id="rId15"/>
+    <sheet name="LongestRowInvisible_Expected" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>dd</t>
   </si>
@@ -200,6 +204,24 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>qq</t>
+  </si>
+  <si>
+    <t>ww</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>rat</t>
+  </si>
+  <si>
+    <t>ddd</t>
   </si>
 </sst>
 </file>
@@ -571,18 +593,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC311C4-AE98-5E43-8D20-4DF34DB89C29}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -607,27 +630,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -791,6 +815,163 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D42D809-2413-7D42-9528-29078949896B}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB789F4-B352-C44A-AC05-1E9CB856ADE9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0685FA5C-3B1B-8B43-A0DE-C31877AC6617}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EC2481-D362-CE42-910F-8498EA2FA4FC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453B851B-2721-4E4B-B8B9-D77A87CF85CE}">
   <dimension ref="A1:B4"/>
@@ -985,7 +1166,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7571C826-D0E5-C441-A8DD-7EE05C8C6CE6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>